<commit_message>
Updated A24_Oscarsa24_released_movies_and_oscars table and SQL query
</commit_message>
<xml_diff>
--- a/A24 Released Movies/A24_Released_Movies_2022_09_17.xlsx
+++ b/A24 Released Movies/A24_Released_Movies_2022_09_17.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexP\Documents\Google Data Analytics Certificate\Case Studies\Case Study 3\A24 Released Movies\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexP\Documents\Google Data Analytics Certificate\Case Studies\Case Study 3\A24 Movies EDA\A24 Released Movies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11547B8-2150-42D1-B69E-6BFE2DC8AD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2FFC8C-5D6B-47D5-9480-19F857C4EAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9977A832-05C3-4F74-B9C5-A7321D2D1C70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="307">
   <si>
     <t>title</t>
   </si>
@@ -954,6 +954,9 @@
   </si>
   <si>
     <t>genre</t>
+  </si>
+  <si>
+    <t>Horror, Psychological, Folk</t>
   </si>
 </sst>
 </file>
@@ -1054,46 +1057,6 @@
   </cellStyles>
   <dxfs count="39">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1174,6 +1137,46 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1230,60 +1233,60 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3788E3AA-75CE-4056-8E12-17D0BB5892EE}" name="Table1" displayName="Table1" ref="A1:J119" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:J119" xr:uid="{3788E3AA-75CE-4056-8E12-17D0BB5892EE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{2FA4FBEC-3311-43D0-92AA-26E9DDC2B7FF}" name="title" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{672ED6CE-7840-4491-8D6B-3AC6BA07950F}" name="release_date" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{29CD66DE-2D9B-482D-915B-827333ACAE25}" name="genre" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{DAF0AE7A-563F-4BB8-8B9C-EF3F18E856F1}" name="director" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{9AA00E7D-A3F2-43C7-BBE7-E2FBD6D96ACC}" name="budget" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{5A5945FE-CF33-4B35-A43E-A70078B00BF5}" name="domestic_revenue" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{EE3AA1C5-F053-4193-9872-F1F6E98D6E0A}" name="international_revenue" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{2770B42E-2BB7-47A0-9A05-196A96E1A9E7}" name="worldwide_revenue" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{2FA4FBEC-3311-43D0-92AA-26E9DDC2B7FF}" name="title" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{672ED6CE-7840-4491-8D6B-3AC6BA07950F}" name="release_date" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{29CD66DE-2D9B-482D-915B-827333ACAE25}" name="genre" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{DAF0AE7A-563F-4BB8-8B9C-EF3F18E856F1}" name="director" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{9AA00E7D-A3F2-43C7-BBE7-E2FBD6D96ACC}" name="budget" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{5A5945FE-CF33-4B35-A43E-A70078B00BF5}" name="domestic_revenue" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{EE3AA1C5-F053-4193-9872-F1F6E98D6E0A}" name="international_revenue" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{2770B42E-2BB7-47A0-9A05-196A96E1A9E7}" name="worldwide_revenue" dataDxfId="26">
       <calculatedColumnFormula>SUM(F2,G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C71D20D0-95E3-4671-A0FA-90C8B995CC6F}" name="runtime" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{232ED58F-9C88-4FA1-AFB5-508A1AF9B67E}" name="MPAA_rating" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{C71D20D0-95E3-4671-A0FA-90C8B995CC6F}" name="runtime" dataDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{232ED58F-9C88-4FA1-AFB5-508A1AF9B67E}" name="MPAA_rating" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5B0D284E-3F84-4C12-B966-5FD9AF49D7CE}" name="Table13" displayName="Table13" ref="A1:J119" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5B0D284E-3F84-4C12-B966-5FD9AF49D7CE}" name="Table13" displayName="Table13" ref="A1:J119" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:J119" xr:uid="{3788E3AA-75CE-4056-8E12-17D0BB5892EE}"/>
   <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{A366D848-955B-4D44-8DC4-285A972557DC}" name="title" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{E103D32C-87AD-409D-8C0E-48164775DE6F}" name="release_date" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{304409B6-B724-4783-B0DF-1CE5D78EA436}" name="genre" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{F45A7276-0179-4620-A1AE-E4AA35BF0651}" name="director" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{37BC62B2-45E7-4899-99FD-A36A384E5CA3}" name="budget" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{B150BCBD-B4AF-4B38-9561-B4D00D3DD1A3}" name="domestic_revenue" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{3F394DDA-36B4-4E22-AF73-860705259100}" name="international_revenue" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{6BEA964C-B517-40BA-AD29-38F780E8C232}" name="worldwide_revenue" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{A366D848-955B-4D44-8DC4-285A972557DC}" name="title" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{E103D32C-87AD-409D-8C0E-48164775DE6F}" name="release_date" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{304409B6-B724-4783-B0DF-1CE5D78EA436}" name="genre" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{F45A7276-0179-4620-A1AE-E4AA35BF0651}" name="director" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{37BC62B2-45E7-4899-99FD-A36A384E5CA3}" name="budget" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{B150BCBD-B4AF-4B38-9561-B4D00D3DD1A3}" name="domestic_revenue" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{3F394DDA-36B4-4E22-AF73-860705259100}" name="international_revenue" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{6BEA964C-B517-40BA-AD29-38F780E8C232}" name="worldwide_revenue" dataDxfId="14">
       <calculatedColumnFormula>SUM(F2,G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2A288A3E-36A5-4CB9-BFB5-1E79B5EF04DC}" name="runtime" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{093312D4-EFD1-4399-B247-055C37FDF467}" name="MPAA_rating" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{2A288A3E-36A5-4CB9-BFB5-1E79B5EF04DC}" name="runtime" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{093312D4-EFD1-4399-B247-055C37FDF467}" name="MPAA_rating" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5DBEB12B-38A5-4C12-84A3-439103211B05}" name="Table134" displayName="Table134" ref="A1:J119" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5DBEB12B-38A5-4C12-84A3-439103211B05}" name="Table134" displayName="Table134" ref="A1:J119" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J119" xr:uid="{3788E3AA-75CE-4056-8E12-17D0BB5892EE}"/>
   <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{2F3E757F-1546-4EA5-ACA7-4CDA708101E8}" name="title" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{2F6F22CF-5398-4458-99F5-DF230DE104D0}" name="release_date" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{4744D67B-E522-4AE1-BE5B-688CCFD70761}" name="genre" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{79F7BFB7-1FA7-42F4-8E68-AA20AD674F3D}" name="director" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{1A0EA7FC-5FF4-4DCC-8F47-DCE7A18F1CFD}" name="budget" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{FA8128C0-CE9D-4BE9-86D4-AA5AA64A9610}" name="domestic_revenue" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{14FE0F0D-2C57-4DCC-B7F4-959E9207CE3C}" name="international_revenue" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{4AFEEB83-544C-44C5-A44C-E0DD63E0E257}" name="worldwide_revenue" dataDxfId="12">
+    <tableColumn id="2" xr3:uid="{2F3E757F-1546-4EA5-ACA7-4CDA708101E8}" name="title" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{2F6F22CF-5398-4458-99F5-DF230DE104D0}" name="release_date" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4744D67B-E522-4AE1-BE5B-688CCFD70761}" name="genre" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{79F7BFB7-1FA7-42F4-8E68-AA20AD674F3D}" name="director" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{1A0EA7FC-5FF4-4DCC-8F47-DCE7A18F1CFD}" name="budget" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FA8128C0-CE9D-4BE9-86D4-AA5AA64A9610}" name="domestic_revenue" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{14FE0F0D-2C57-4DCC-B7F4-959E9207CE3C}" name="international_revenue" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4AFEEB83-544C-44C5-A44C-E0DD63E0E257}" name="worldwide_revenue" dataDxfId="2">
       <calculatedColumnFormula>SUM(F2,G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{36A6BDE5-CB97-484B-AC4A-FA811FFE3C26}" name="runtime" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{7104473B-0191-4578-A0E3-CF662AAE763B}" name="MPAA_rating" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{36A6BDE5-CB97-484B-AC4A-FA811FFE3C26}" name="runtime" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{7104473B-0191-4578-A0E3-CF662AAE763B}" name="MPAA_rating" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1589,10 +1592,10 @@
   <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A44" sqref="A44"/>
+      <selection pane="bottomRight" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3121,7 +3124,7 @@
         <v>44701</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>146</v>

</xml_diff>